<commit_message>
Add AutoSkl1 test results
</commit_message>
<xml_diff>
--- a/Test_Results.xlsx
+++ b/Test_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nevadaunr-my.sharepoint.com/personal/nalvarez_nevada_unr_edu/Documents/2022 Spring/CS791 - High Performance Computing/Project/cs791/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="8_{40405BED-1EE5-4A7E-B8AC-C33E5F50C249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7285F92B-687B-40E0-B963-B4FCC7A8D6D2}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="8_{40405BED-1EE5-4A7E-B8AC-C33E5F50C249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4560EF96-CBB6-4CEB-BC07-41E87874A7B4}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4860" windowWidth="29040" windowHeight="15840" xr2:uid="{DAF91758-B7D5-4BA4-9138-01558502D7C9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Model</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>LinearSVC(C=0.25, dual=False, penalty='l1', tol=1e-05)</t>
+  </si>
+  <si>
+    <t>AutoSklearn - 60 seconds - 4 cores - 3GB RAM</t>
   </si>
 </sst>
 </file>
@@ -448,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE89014-BA59-4F10-967A-38B305765E4C}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,301 +494,332 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>0.98518518518518505</v>
+        <v>0.99166666666666603</v>
       </c>
       <c r="D2" s="4">
-        <f>4*60+2-8</f>
-        <v>234</v>
+        <f>1*60+10</f>
+        <v>70</v>
       </c>
       <c r="E2" s="4">
+        <v>72</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.66518518518518499</v>
+      </c>
+      <c r="G2" s="4">
+        <f>1*60+5</f>
+        <v>65</v>
+      </c>
+      <c r="H2" s="4">
         <v>8</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.66444444444444395</v>
-      </c>
-      <c r="G2" s="4">
-        <f>1*60+32-7</f>
-        <v>85</v>
-      </c>
-      <c r="H2" s="4">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>0.45648148148148099</v>
+        <v>0.99166666670000003</v>
       </c>
       <c r="D3" s="4">
-        <f>2*60-11</f>
-        <v>109</v>
+        <f>3*60</f>
+        <v>180</v>
       </c>
       <c r="E3" s="4">
+        <v>322</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.66703703703703698</v>
+      </c>
+      <c r="G3" s="4">
+        <f>2*60+10-8</f>
+        <v>122</v>
+      </c>
+      <c r="H3" s="4">
         <v>11</v>
       </c>
-      <c r="F3" s="1">
-        <v>0.45740740740740699</v>
-      </c>
-      <c r="G3" s="4">
-        <f>1*60+30-7</f>
-        <v>83</v>
-      </c>
-      <c r="H3" s="4">
-        <v>7</v>
+      <c r="I3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>0.98240740740740695</v>
+        <v>0.162962962962962</v>
       </c>
       <c r="D4" s="4">
-        <f>1*60+39-12</f>
-        <v>87</v>
+        <f>3*60</f>
+        <v>180</v>
       </c>
       <c r="E4" s="4">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="F4" s="1">
-        <v>0.35111111111111099</v>
+        <v>0.16666666666666599</v>
       </c>
       <c r="G4" s="4">
-        <f>2*60+46-7</f>
-        <v>159</v>
+        <f>2*60+10-8</f>
+        <v>122</v>
       </c>
       <c r="H4" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>0.162962962962962</v>
+        <v>0.99166666670000003</v>
       </c>
       <c r="D5" s="4">
         <f>3*60</f>
         <v>180</v>
       </c>
       <c r="E5" s="4">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F5" s="1">
-        <v>0.16666666666666599</v>
+        <v>0.66703703703703698</v>
       </c>
       <c r="G5" s="4">
         <f>2*60+10-8</f>
         <v>122</v>
       </c>
       <c r="H5" s="4">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
       <c r="C6" s="1">
-        <v>0.99166666670000003</v>
+        <v>0.98240740740740695</v>
       </c>
       <c r="D6" s="4">
-        <f>3*60</f>
-        <v>180</v>
+        <f>1*60+39-12</f>
+        <v>87</v>
       </c>
       <c r="E6" s="4">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1">
-        <v>0.66703703703703698</v>
+        <v>0.35111111111111099</v>
       </c>
       <c r="G6" s="4">
-        <f>2*60+10-8</f>
-        <v>122</v>
+        <f>2*60+46-7</f>
+        <v>159</v>
       </c>
       <c r="H6" s="4">
-        <v>11</v>
-      </c>
-      <c r="I6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>0.99166666670000003</v>
+        <v>0.98425925925925895</v>
       </c>
       <c r="D7" s="4">
-        <f>3*60</f>
-        <v>180</v>
+        <f>1*60+39-12+18*60+5-7</f>
+        <v>1165</v>
       </c>
       <c r="E7" s="4">
-        <v>322</v>
+        <f>9</f>
+        <v>9</v>
       </c>
       <c r="F7" s="1">
-        <v>0.66703703703703698</v>
+        <v>0.45407407407407402</v>
       </c>
       <c r="G7" s="4">
-        <f>2*60+10-8</f>
-        <v>122</v>
+        <f>2*60+46-7</f>
+        <v>159</v>
       </c>
       <c r="H7" s="4">
-        <v>11</v>
-      </c>
-      <c r="I7" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1">
-        <v>0.98425925925925895</v>
+        <v>0.56018518518518501</v>
       </c>
       <c r="D8" s="4">
-        <f>1*60+39-12+18*60+5-7</f>
-        <v>1165</v>
+        <f>1*60+12</f>
+        <v>72</v>
       </c>
       <c r="E8" s="4">
-        <f>9</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F8" s="1">
-        <v>0.45407407407407402</v>
+        <v>0.45740740740740699</v>
       </c>
       <c r="G8" s="4">
-        <f>2*60+46-7</f>
-        <v>159</v>
+        <f>1*60+10</f>
+        <v>70</v>
       </c>
       <c r="H8" s="4">
         <v>7</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
       </c>
       <c r="C9" s="1">
+        <v>0.99351851851851802</v>
+      </c>
+      <c r="D9" s="4">
+        <f>1*60+12+3*60+45</f>
+        <v>297</v>
+      </c>
+      <c r="E9" s="4">
+        <v>25</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.31037037037037002</v>
+      </c>
+      <c r="G9" s="4">
+        <f>1*60+10</f>
+        <v>70</v>
+      </c>
+      <c r="H9" s="4">
+        <v>7</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.98518518518518505</v>
+      </c>
+      <c r="D10" s="4">
+        <f>4*60+2-8</f>
+        <v>234</v>
+      </c>
+      <c r="E10" s="4">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.66444444444444395</v>
+      </c>
+      <c r="G10" s="4">
+        <f>1*60+32-7</f>
+        <v>85</v>
+      </c>
+      <c r="H10" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
         <v>0.98703703703703705</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D11" s="4">
         <f>4*60+2-8+5*60+53-22</f>
         <v>565</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E11" s="4">
         <v>22</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F11" s="1">
         <v>0.66518518518518499</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G11" s="4">
         <f>1*60+32-7</f>
         <v>85</v>
       </c>
-      <c r="H9" s="4">
-        <v>7</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.56018518518518501</v>
-      </c>
-      <c r="D10" s="4">
-        <f>1*60+12</f>
-        <v>72</v>
-      </c>
-      <c r="E10" s="4">
-        <v>13</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.45740740740740699</v>
-      </c>
-      <c r="G10" s="4">
-        <f>1*60+10</f>
-        <v>70</v>
-      </c>
-      <c r="H10" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.99351851851851802</v>
-      </c>
-      <c r="D11" s="4">
-        <f>1*60+12+3*60+45</f>
-        <v>297</v>
-      </c>
-      <c r="E11" s="4">
-        <v>25</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0.31037037037037002</v>
-      </c>
-      <c r="G11" s="4">
-        <f>1*60+10</f>
-        <v>70</v>
-      </c>
       <c r="H11" s="4">
         <v>7</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.45648148148148099</v>
+      </c>
+      <c r="D12" s="4">
+        <f>2*60-11</f>
+        <v>109</v>
+      </c>
+      <c r="E12" s="4">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.45740740740740699</v>
+      </c>
+      <c r="G12" s="4">
+        <f>1*60+30-7</f>
+        <v>83</v>
+      </c>
+      <c r="H12" s="4">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I12">
+    <sortCondition ref="A2:A12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>